<commit_message>
Change project name to com.lockedme
</commit_message>
<xml_diff>
--- a/LockedMe.com - Product and Sprint Backlog.xlsx
+++ b/LockedMe.com - Product and Sprint Backlog.xlsx
@@ -275,7 +275,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -321,18 +321,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFEDEDF0"/>
-        <bgColor rgb="FFEDEDF0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFEDEDF0"/>
       </patternFill>
     </fill>
@@ -417,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -573,56 +561,8 @@
     <xf numFmtId="166" fontId="8" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="6" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -630,9 +570,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -676,6 +613,52 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -978,7 +961,7 @@
   <dimension ref="A1:R528"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
@@ -1009,20 +992,20 @@
     </row>
     <row r="2" spans="1:18" ht="52.5" customHeight="1" thickBot="1">
       <c r="A2" s="53"/>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
       <c r="N2" s="57"/>
       <c r="O2" s="57"/>
       <c r="P2" s="57"/>
@@ -1051,20 +1034,20 @@
     </row>
     <row r="4" spans="1:18" ht="34.5" customHeight="1">
       <c r="A4" s="4"/>
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="84" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="64"/>
-      <c r="K4" s="64"/>
-      <c r="L4" s="64"/>
-      <c r="M4" s="64"/>
+      <c r="C4" s="85"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
+      <c r="I4" s="85"/>
+      <c r="J4" s="85"/>
+      <c r="K4" s="85"/>
+      <c r="L4" s="85"/>
+      <c r="M4" s="85"/>
       <c r="N4" s="59"/>
       <c r="O4" s="59"/>
       <c r="P4" s="59"/>
@@ -1090,11 +1073,11 @@
     </row>
     <row r="6" spans="1:18" ht="15" customHeight="1">
       <c r="A6" s="2"/>
-      <c r="B6" s="65" t="s">
+      <c r="B6" s="86" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -1112,9 +1095,9 @@
     </row>
     <row r="7" spans="1:18" ht="15" customHeight="1">
       <c r="A7" s="2"/>
-      <c r="B7" s="65"/>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
+      <c r="B7" s="86"/>
+      <c r="C7" s="86"/>
+      <c r="D7" s="86"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -1132,17 +1115,17 @@
     </row>
     <row r="8" spans="1:18" ht="15" customHeight="1">
       <c r="A8" s="2"/>
-      <c r="B8" s="61" t="s">
+      <c r="B8" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61"/>
-      <c r="G8" s="61"/>
-      <c r="H8" s="61"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="61"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="82"/>
+      <c r="E8" s="82"/>
+      <c r="F8" s="82"/>
+      <c r="G8" s="82"/>
+      <c r="H8" s="82"/>
+      <c r="I8" s="82"/>
+      <c r="J8" s="82"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="54"/>
@@ -1154,15 +1137,15 @@
     </row>
     <row r="9" spans="1:18" ht="15" customHeight="1">
       <c r="A9" s="2"/>
-      <c r="B9" s="61"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="61"/>
-      <c r="H9" s="61"/>
-      <c r="I9" s="61"/>
-      <c r="J9" s="61"/>
+      <c r="B9" s="82"/>
+      <c r="C9" s="82"/>
+      <c r="D9" s="82"/>
+      <c r="E9" s="82"/>
+      <c r="F9" s="82"/>
+      <c r="G9" s="82"/>
+      <c r="H9" s="82"/>
+      <c r="I9" s="82"/>
+      <c r="J9" s="82"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="54"/>
@@ -1174,15 +1157,15 @@
     </row>
     <row r="10" spans="1:18" ht="15" customHeight="1">
       <c r="A10" s="2"/>
-      <c r="B10" s="61"/>
-      <c r="C10" s="61"/>
-      <c r="D10" s="61"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="61"/>
-      <c r="H10" s="61"/>
-      <c r="I10" s="61"/>
-      <c r="J10" s="61"/>
+      <c r="B10" s="82"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="82"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="82"/>
+      <c r="G10" s="82"/>
+      <c r="H10" s="82"/>
+      <c r="I10" s="82"/>
+      <c r="J10" s="82"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="54"/>
@@ -1194,15 +1177,15 @@
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1">
       <c r="A11" s="2"/>
-      <c r="B11" s="61"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="61"/>
-      <c r="I11" s="61"/>
-      <c r="J11" s="61"/>
+      <c r="B11" s="82"/>
+      <c r="C11" s="82"/>
+      <c r="D11" s="82"/>
+      <c r="E11" s="82"/>
+      <c r="F11" s="82"/>
+      <c r="G11" s="82"/>
+      <c r="H11" s="82"/>
+      <c r="I11" s="82"/>
+      <c r="J11" s="82"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11" s="54"/>
@@ -1214,15 +1197,15 @@
     </row>
     <row r="12" spans="1:18" ht="15" customHeight="1">
       <c r="A12" s="2"/>
-      <c r="B12" s="61"/>
-      <c r="C12" s="61"/>
-      <c r="D12" s="61"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="61"/>
-      <c r="H12" s="61"/>
-      <c r="I12" s="61"/>
-      <c r="J12" s="61"/>
+      <c r="B12" s="82"/>
+      <c r="C12" s="82"/>
+      <c r="D12" s="82"/>
+      <c r="E12" s="82"/>
+      <c r="F12" s="82"/>
+      <c r="G12" s="82"/>
+      <c r="H12" s="82"/>
+      <c r="I12" s="82"/>
+      <c r="J12" s="82"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="54"/>
@@ -1234,15 +1217,15 @@
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1">
       <c r="A13" s="2"/>
-      <c r="B13" s="61"/>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="61"/>
-      <c r="H13" s="61"/>
-      <c r="I13" s="61"/>
-      <c r="J13" s="61"/>
+      <c r="B13" s="82"/>
+      <c r="C13" s="82"/>
+      <c r="D13" s="82"/>
+      <c r="E13" s="82"/>
+      <c r="F13" s="82"/>
+      <c r="G13" s="82"/>
+      <c r="H13" s="82"/>
+      <c r="I13" s="82"/>
+      <c r="J13" s="82"/>
       <c r="L13" s="2"/>
       <c r="M13" s="55"/>
       <c r="N13" s="58"/>
@@ -1267,20 +1250,20 @@
     </row>
     <row r="15" spans="1:18" ht="34.5" customHeight="1">
       <c r="A15" s="4"/>
-      <c r="B15" s="63" t="s">
+      <c r="B15" s="84" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="64"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="64"/>
-      <c r="H15" s="64"/>
-      <c r="I15" s="64"/>
-      <c r="J15" s="64"/>
-      <c r="K15" s="64"/>
-      <c r="L15" s="64"/>
-      <c r="M15" s="64"/>
+      <c r="C15" s="85"/>
+      <c r="D15" s="85"/>
+      <c r="E15" s="85"/>
+      <c r="F15" s="85"/>
+      <c r="G15" s="85"/>
+      <c r="H15" s="85"/>
+      <c r="I15" s="85"/>
+      <c r="J15" s="85"/>
+      <c r="K15" s="85"/>
+      <c r="L15" s="85"/>
+      <c r="M15" s="85"/>
       <c r="N15" s="59"/>
       <c r="O15" s="59"/>
       <c r="P15" s="59"/>
@@ -1329,28 +1312,28 @@
     </row>
     <row r="18" spans="1:18" ht="39" customHeight="1">
       <c r="A18" s="9"/>
-      <c r="B18" s="84" t="s">
+      <c r="B18" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="84" t="s">
+      <c r="C18" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="84" t="s">
+      <c r="D18" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="84" t="s">
+      <c r="E18" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="84" t="s">
+      <c r="F18" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="G18" s="84" t="s">
+      <c r="G18" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="H18" s="84" t="s">
+      <c r="H18" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="I18" s="84" t="s">
+      <c r="I18" s="62" t="s">
         <v>10</v>
       </c>
       <c r="J18" s="10"/>
@@ -10588,7 +10571,7 @@
     <mergeCell ref="B6:D7"/>
   </mergeCells>
   <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
-  <pageSetup fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="48" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -10600,9 +10583,7 @@
   </sheetPr>
   <dimension ref="A1:N552"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -10621,21 +10602,21 @@
     <row r="1" spans="1:14" ht="40.5" customHeight="1"/>
     <row r="2" spans="1:14" ht="52.5" customHeight="1" thickBot="1">
       <c r="A2" s="53"/>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
-      <c r="N2" s="62"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="83"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1">
       <c r="A3" s="1"/>
@@ -10653,47 +10634,47 @@
     </row>
     <row r="4" spans="1:14" ht="34.5" customHeight="1">
       <c r="A4" s="4"/>
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="87" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
-      <c r="J4" s="73"/>
-      <c r="K4" s="73"/>
-      <c r="L4" s="73"/>
-      <c r="M4" s="73"/>
-      <c r="N4" s="73"/>
+      <c r="C4" s="87"/>
+      <c r="D4" s="87"/>
+      <c r="E4" s="87"/>
+      <c r="F4" s="87"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="87"/>
+      <c r="K4" s="87"/>
+      <c r="L4" s="87"/>
+      <c r="M4" s="87"/>
+      <c r="N4" s="87"/>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1">
       <c r="A5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="85"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="85"/>
-      <c r="J5" s="86"/>
-      <c r="K5" s="85"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="64"/>
+      <c r="K5" s="63"/>
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:14" ht="30.75" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="74" t="s">
+      <c r="B6" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="74"/>
-      <c r="D6" s="74"/>
+      <c r="C6" s="95"/>
+      <c r="D6" s="95"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="87"/>
-      <c r="G6" s="88"/>
-      <c r="H6" s="88"/>
-      <c r="I6" s="88"/>
-      <c r="J6" s="88"/>
-      <c r="K6" s="88"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="96"/>
+      <c r="H6" s="96"/>
+      <c r="I6" s="96"/>
+      <c r="J6" s="96"/>
+      <c r="K6" s="96"/>
       <c r="L6" s="1"/>
     </row>
     <row r="7" spans="1:14" ht="32.25" customHeight="1">
@@ -10702,135 +10683,135 @@
       <c r="C7" s="6"/>
       <c r="D7" s="7"/>
       <c r="E7" s="6"/>
-      <c r="F7" s="85"/>
-      <c r="G7" s="85"/>
-      <c r="H7" s="85"/>
-      <c r="I7" s="87"/>
-      <c r="J7" s="87"/>
-      <c r="K7" s="87"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="65"/>
+      <c r="K7" s="65"/>
       <c r="L7" s="5"/>
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="66" t="s">
+      <c r="B8" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="67"/>
+      <c r="C8" s="89"/>
       <c r="D8" s="39">
         <v>14</v>
       </c>
-      <c r="F8" s="87"/>
-      <c r="G8" s="87"/>
-      <c r="H8" s="87"/>
-      <c r="I8" s="87"/>
-      <c r="J8" s="87"/>
-      <c r="K8" s="87"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="65"/>
+      <c r="H8" s="65"/>
+      <c r="I8" s="65"/>
+      <c r="J8" s="65"/>
+      <c r="K8" s="65"/>
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="66" t="s">
+      <c r="B9" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="67"/>
+      <c r="C9" s="89"/>
       <c r="D9" s="40">
         <v>0</v>
       </c>
-      <c r="F9" s="85"/>
-      <c r="G9" s="89"/>
-      <c r="H9" s="87"/>
-      <c r="I9" s="87"/>
-      <c r="J9" s="87"/>
-      <c r="K9" s="87"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="65"/>
+      <c r="I9" s="65"/>
+      <c r="J9" s="65"/>
+      <c r="K9" s="65"/>
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:14" ht="15" customHeight="1">
       <c r="A10" s="1"/>
-      <c r="B10" s="68" t="s">
+      <c r="B10" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="69"/>
+      <c r="C10" s="91"/>
       <c r="D10" s="39">
         <v>14</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="85"/>
-      <c r="G10" s="85"/>
-      <c r="H10" s="85"/>
-      <c r="I10" s="87"/>
-      <c r="J10" s="87"/>
-      <c r="K10" s="87"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="63"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="65"/>
+      <c r="J10" s="65"/>
+      <c r="K10" s="65"/>
       <c r="L10" s="1"/>
     </row>
     <row r="11" spans="1:14" ht="15" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="71"/>
-      <c r="C11" s="72"/>
+      <c r="B11" s="93"/>
+      <c r="C11" s="94"/>
       <c r="D11" s="41"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="85"/>
-      <c r="G11" s="85"/>
-      <c r="H11" s="85"/>
-      <c r="I11" s="87"/>
-      <c r="J11" s="87"/>
-      <c r="K11" s="87"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="65"/>
+      <c r="J11" s="65"/>
+      <c r="K11" s="65"/>
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:14" ht="15" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="70" t="s">
+      <c r="B12" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="70"/>
+      <c r="C12" s="92"/>
       <c r="D12" s="42">
         <f>1-(D8/D10)</f>
         <v>0</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="85"/>
-      <c r="G12" s="85"/>
-      <c r="H12" s="85"/>
-      <c r="I12" s="87"/>
-      <c r="J12" s="87"/>
-      <c r="K12" s="87"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="63"/>
+      <c r="H12" s="63"/>
+      <c r="I12" s="65"/>
+      <c r="J12" s="65"/>
+      <c r="K12" s="65"/>
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:14" ht="15" customHeight="1">
       <c r="A13" s="1"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="85"/>
-      <c r="G13" s="85"/>
-      <c r="H13" s="85"/>
-      <c r="I13" s="87"/>
-      <c r="J13" s="87"/>
-      <c r="K13" s="87"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="65"/>
+      <c r="J13" s="65"/>
+      <c r="K13" s="65"/>
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:14" ht="15" customHeight="1">
       <c r="A14" s="1"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="85"/>
-      <c r="G14" s="85"/>
-      <c r="H14" s="85"/>
-      <c r="I14" s="87"/>
-      <c r="J14" s="87"/>
-      <c r="K14" s="87"/>
+      <c r="F14" s="63"/>
+      <c r="G14" s="63"/>
+      <c r="H14" s="63"/>
+      <c r="I14" s="65"/>
+      <c r="J14" s="65"/>
+      <c r="K14" s="65"/>
       <c r="L14" s="1"/>
     </row>
     <row r="15" spans="1:14" ht="15.75">
       <c r="A15" s="1"/>
-      <c r="F15" s="87"/>
-      <c r="G15" s="91"/>
-      <c r="H15" s="90"/>
-      <c r="I15" s="90"/>
-      <c r="J15" s="90"/>
-      <c r="K15" s="90"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="68"/>
+      <c r="H15" s="67"/>
+      <c r="I15" s="67"/>
+      <c r="J15" s="67"/>
+      <c r="K15" s="67"/>
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:14" ht="15" customHeight="1">
       <c r="A16" s="1"/>
-      <c r="D16" s="103"/>
-      <c r="E16" s="104"/>
+      <c r="D16" s="80"/>
+      <c r="E16" s="81"/>
       <c r="F16" s="1"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -10846,21 +10827,21 @@
     </row>
     <row r="18" spans="1:14" ht="34.5" customHeight="1">
       <c r="A18" s="4"/>
-      <c r="B18" s="73" t="s">
+      <c r="B18" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="73"/>
-      <c r="D18" s="73"/>
-      <c r="E18" s="73"/>
-      <c r="F18" s="73"/>
-      <c r="G18" s="73"/>
-      <c r="H18" s="73"/>
-      <c r="I18" s="73"/>
-      <c r="J18" s="73"/>
-      <c r="K18" s="73"/>
-      <c r="L18" s="73"/>
-      <c r="M18" s="73"/>
-      <c r="N18" s="73"/>
+      <c r="C18" s="87"/>
+      <c r="D18" s="87"/>
+      <c r="E18" s="87"/>
+      <c r="F18" s="87"/>
+      <c r="G18" s="87"/>
+      <c r="H18" s="87"/>
+      <c r="I18" s="87"/>
+      <c r="J18" s="87"/>
+      <c r="K18" s="87"/>
+      <c r="L18" s="87"/>
+      <c r="M18" s="87"/>
+      <c r="N18" s="87"/>
     </row>
     <row r="19" spans="1:14" ht="15" customHeight="1">
       <c r="A19" s="1"/>
@@ -11039,18 +11020,18 @@
       <c r="J26" s="28"/>
       <c r="K26" s="29"/>
     </row>
-    <row r="27" spans="1:14" s="82" customFormat="1" ht="15" customHeight="1">
-      <c r="A27" s="75"/>
-      <c r="B27" s="76"/>
-      <c r="C27" s="77"/>
-      <c r="D27" s="77"/>
-      <c r="E27" s="78"/>
-      <c r="F27" s="79"/>
-      <c r="G27" s="78"/>
-      <c r="H27" s="77"/>
-      <c r="I27" s="77"/>
-      <c r="J27" s="80"/>
-      <c r="K27" s="81"/>
+    <row r="27" spans="1:14" s="61" customFormat="1" ht="15" customHeight="1">
+      <c r="A27" s="69"/>
+      <c r="B27" s="70"/>
+      <c r="C27" s="97"/>
+      <c r="D27" s="97"/>
+      <c r="E27" s="98"/>
+      <c r="F27" s="99"/>
+      <c r="G27" s="98"/>
+      <c r="H27" s="97"/>
+      <c r="I27" s="97"/>
+      <c r="J27" s="100"/>
+      <c r="K27" s="101"/>
     </row>
     <row r="28" spans="1:14" ht="102.75" customHeight="1">
       <c r="A28" s="13"/>
@@ -11275,161 +11256,161 @@
       <c r="J36" s="28"/>
       <c r="K36" s="29"/>
     </row>
-    <row r="37" spans="1:11" s="83" customFormat="1" ht="15.75">
-      <c r="A37" s="92"/>
-      <c r="B37" s="93"/>
-      <c r="C37" s="94"/>
-      <c r="D37" s="94"/>
-      <c r="E37" s="95"/>
-      <c r="F37" s="96"/>
-      <c r="G37" s="95"/>
-      <c r="H37" s="94"/>
-      <c r="I37" s="94"/>
-      <c r="J37" s="97"/>
-      <c r="K37" s="98"/>
-    </row>
-    <row r="38" spans="1:11" s="83" customFormat="1" ht="15" customHeight="1">
-      <c r="A38" s="92"/>
-      <c r="B38" s="93"/>
-      <c r="C38" s="94"/>
-      <c r="D38" s="94"/>
-      <c r="E38" s="95"/>
-      <c r="F38" s="96"/>
-      <c r="G38" s="95"/>
-      <c r="H38" s="94"/>
-      <c r="I38" s="94"/>
-      <c r="J38" s="97"/>
-      <c r="K38" s="98"/>
-    </row>
-    <row r="39" spans="1:11" s="83" customFormat="1" ht="15.75">
-      <c r="A39" s="92"/>
-      <c r="B39" s="93"/>
-      <c r="C39" s="99"/>
-      <c r="D39" s="100"/>
-      <c r="E39" s="101"/>
-      <c r="F39" s="93"/>
-      <c r="G39" s="101"/>
-      <c r="H39" s="101"/>
-      <c r="I39" s="101"/>
-      <c r="J39" s="101"/>
-      <c r="K39" s="102"/>
-    </row>
-    <row r="40" spans="1:11" s="83" customFormat="1" ht="15" customHeight="1">
-      <c r="A40" s="92"/>
-      <c r="B40" s="93"/>
-      <c r="C40" s="94"/>
-      <c r="D40" s="94"/>
-      <c r="E40" s="95"/>
-      <c r="F40" s="96"/>
-      <c r="G40" s="95"/>
-      <c r="H40" s="94"/>
-      <c r="I40" s="94"/>
-      <c r="J40" s="97"/>
-      <c r="K40" s="98"/>
-    </row>
-    <row r="41" spans="1:11" s="83" customFormat="1" ht="15" customHeight="1">
-      <c r="A41" s="92"/>
-      <c r="B41" s="93"/>
-      <c r="C41" s="94"/>
-      <c r="D41" s="94"/>
-      <c r="E41" s="95"/>
-      <c r="F41" s="96"/>
-      <c r="G41" s="95"/>
-      <c r="H41" s="94"/>
-      <c r="I41" s="94"/>
-      <c r="J41" s="97"/>
-      <c r="K41" s="98"/>
-    </row>
-    <row r="42" spans="1:11" s="83" customFormat="1" ht="15" customHeight="1">
-      <c r="A42" s="92"/>
-      <c r="B42" s="93"/>
-      <c r="C42" s="94"/>
-      <c r="D42" s="94"/>
-      <c r="E42" s="95"/>
-      <c r="F42" s="96"/>
-      <c r="G42" s="95"/>
-      <c r="H42" s="94"/>
-      <c r="I42" s="94"/>
-      <c r="J42" s="97"/>
-      <c r="K42" s="98"/>
-    </row>
-    <row r="43" spans="1:11" s="83" customFormat="1" ht="15.75">
-      <c r="A43" s="92"/>
-      <c r="B43" s="93"/>
-      <c r="C43" s="94"/>
-      <c r="D43" s="94"/>
-      <c r="E43" s="95"/>
-      <c r="F43" s="96"/>
-      <c r="G43" s="95"/>
-      <c r="H43" s="94"/>
-      <c r="I43" s="94"/>
-      <c r="J43" s="97"/>
-      <c r="K43" s="98"/>
-    </row>
-    <row r="44" spans="1:11" s="83" customFormat="1" ht="15.75">
-      <c r="A44" s="92"/>
-      <c r="B44" s="93"/>
-      <c r="C44" s="99"/>
-      <c r="D44" s="100"/>
-      <c r="E44" s="101"/>
-      <c r="F44" s="93"/>
-      <c r="G44" s="101"/>
-      <c r="H44" s="101"/>
-      <c r="I44" s="101"/>
-      <c r="J44" s="101"/>
-      <c r="K44" s="102"/>
-    </row>
-    <row r="45" spans="1:11" s="83" customFormat="1" ht="15" customHeight="1">
-      <c r="A45" s="92"/>
-      <c r="B45" s="93"/>
-      <c r="C45" s="94"/>
-      <c r="D45" s="94"/>
-      <c r="E45" s="95"/>
-      <c r="F45" s="96"/>
-      <c r="G45" s="95"/>
-      <c r="H45" s="94"/>
-      <c r="I45" s="94"/>
-      <c r="J45" s="97"/>
-      <c r="K45" s="98"/>
-    </row>
-    <row r="46" spans="1:11" s="83" customFormat="1" ht="15" customHeight="1">
-      <c r="A46" s="92"/>
-      <c r="B46" s="93"/>
-      <c r="C46" s="94"/>
-      <c r="D46" s="94"/>
-      <c r="E46" s="95"/>
-      <c r="F46" s="96"/>
-      <c r="G46" s="95"/>
-      <c r="H46" s="94"/>
-      <c r="I46" s="94"/>
-      <c r="J46" s="97"/>
-      <c r="K46" s="98"/>
-    </row>
-    <row r="47" spans="1:11" s="83" customFormat="1" ht="15" customHeight="1">
-      <c r="A47" s="92"/>
-      <c r="B47" s="93"/>
-      <c r="C47" s="94"/>
-      <c r="D47" s="94"/>
-      <c r="E47" s="95"/>
-      <c r="F47" s="96"/>
-      <c r="G47" s="95"/>
-      <c r="H47" s="94"/>
-      <c r="I47" s="94"/>
-      <c r="J47" s="97"/>
-      <c r="K47" s="98"/>
-    </row>
-    <row r="48" spans="1:11" s="83" customFormat="1" ht="15" customHeight="1">
-      <c r="A48" s="92"/>
-      <c r="B48" s="93"/>
-      <c r="C48" s="94"/>
-      <c r="D48" s="94"/>
-      <c r="E48" s="95"/>
-      <c r="F48" s="96"/>
-      <c r="G48" s="95"/>
-      <c r="H48" s="94"/>
-      <c r="I48" s="94"/>
-      <c r="J48" s="97"/>
-      <c r="K48" s="98"/>
+    <row r="37" spans="1:11" s="61" customFormat="1" ht="15.75">
+      <c r="A37" s="69"/>
+      <c r="B37" s="70"/>
+      <c r="C37" s="71"/>
+      <c r="D37" s="71"/>
+      <c r="E37" s="72"/>
+      <c r="F37" s="73"/>
+      <c r="G37" s="72"/>
+      <c r="H37" s="71"/>
+      <c r="I37" s="71"/>
+      <c r="J37" s="74"/>
+      <c r="K37" s="75"/>
+    </row>
+    <row r="38" spans="1:11" s="61" customFormat="1" ht="15" customHeight="1">
+      <c r="A38" s="69"/>
+      <c r="B38" s="70"/>
+      <c r="C38" s="71"/>
+      <c r="D38" s="71"/>
+      <c r="E38" s="72"/>
+      <c r="F38" s="73"/>
+      <c r="G38" s="72"/>
+      <c r="H38" s="71"/>
+      <c r="I38" s="71"/>
+      <c r="J38" s="74"/>
+      <c r="K38" s="75"/>
+    </row>
+    <row r="39" spans="1:11" s="61" customFormat="1" ht="15.75">
+      <c r="A39" s="69"/>
+      <c r="B39" s="70"/>
+      <c r="C39" s="76"/>
+      <c r="D39" s="77"/>
+      <c r="E39" s="78"/>
+      <c r="F39" s="70"/>
+      <c r="G39" s="78"/>
+      <c r="H39" s="78"/>
+      <c r="I39" s="78"/>
+      <c r="J39" s="78"/>
+      <c r="K39" s="79"/>
+    </row>
+    <row r="40" spans="1:11" s="61" customFormat="1" ht="15" customHeight="1">
+      <c r="A40" s="69"/>
+      <c r="B40" s="70"/>
+      <c r="C40" s="71"/>
+      <c r="D40" s="71"/>
+      <c r="E40" s="72"/>
+      <c r="F40" s="73"/>
+      <c r="G40" s="72"/>
+      <c r="H40" s="71"/>
+      <c r="I40" s="71"/>
+      <c r="J40" s="74"/>
+      <c r="K40" s="75"/>
+    </row>
+    <row r="41" spans="1:11" s="61" customFormat="1" ht="15" customHeight="1">
+      <c r="A41" s="69"/>
+      <c r="B41" s="70"/>
+      <c r="C41" s="71"/>
+      <c r="D41" s="71"/>
+      <c r="E41" s="72"/>
+      <c r="F41" s="73"/>
+      <c r="G41" s="72"/>
+      <c r="H41" s="71"/>
+      <c r="I41" s="71"/>
+      <c r="J41" s="74"/>
+      <c r="K41" s="75"/>
+    </row>
+    <row r="42" spans="1:11" s="61" customFormat="1" ht="15" customHeight="1">
+      <c r="A42" s="69"/>
+      <c r="B42" s="70"/>
+      <c r="C42" s="71"/>
+      <c r="D42" s="71"/>
+      <c r="E42" s="72"/>
+      <c r="F42" s="73"/>
+      <c r="G42" s="72"/>
+      <c r="H42" s="71"/>
+      <c r="I42" s="71"/>
+      <c r="J42" s="74"/>
+      <c r="K42" s="75"/>
+    </row>
+    <row r="43" spans="1:11" s="61" customFormat="1" ht="15.75">
+      <c r="A43" s="69"/>
+      <c r="B43" s="70"/>
+      <c r="C43" s="71"/>
+      <c r="D43" s="71"/>
+      <c r="E43" s="72"/>
+      <c r="F43" s="73"/>
+      <c r="G43" s="72"/>
+      <c r="H43" s="71"/>
+      <c r="I43" s="71"/>
+      <c r="J43" s="74"/>
+      <c r="K43" s="75"/>
+    </row>
+    <row r="44" spans="1:11" s="61" customFormat="1" ht="15.75">
+      <c r="A44" s="69"/>
+      <c r="B44" s="70"/>
+      <c r="C44" s="76"/>
+      <c r="D44" s="77"/>
+      <c r="E44" s="78"/>
+      <c r="F44" s="70"/>
+      <c r="G44" s="78"/>
+      <c r="H44" s="78"/>
+      <c r="I44" s="78"/>
+      <c r="J44" s="78"/>
+      <c r="K44" s="79"/>
+    </row>
+    <row r="45" spans="1:11" s="61" customFormat="1" ht="15" customHeight="1">
+      <c r="A45" s="69"/>
+      <c r="B45" s="70"/>
+      <c r="C45" s="71"/>
+      <c r="D45" s="71"/>
+      <c r="E45" s="72"/>
+      <c r="F45" s="73"/>
+      <c r="G45" s="72"/>
+      <c r="H45" s="71"/>
+      <c r="I45" s="71"/>
+      <c r="J45" s="74"/>
+      <c r="K45" s="75"/>
+    </row>
+    <row r="46" spans="1:11" s="61" customFormat="1" ht="15" customHeight="1">
+      <c r="A46" s="69"/>
+      <c r="B46" s="70"/>
+      <c r="C46" s="71"/>
+      <c r="D46" s="71"/>
+      <c r="E46" s="72"/>
+      <c r="F46" s="73"/>
+      <c r="G46" s="72"/>
+      <c r="H46" s="71"/>
+      <c r="I46" s="71"/>
+      <c r="J46" s="74"/>
+      <c r="K46" s="75"/>
+    </row>
+    <row r="47" spans="1:11" s="61" customFormat="1" ht="15" customHeight="1">
+      <c r="A47" s="69"/>
+      <c r="B47" s="70"/>
+      <c r="C47" s="71"/>
+      <c r="D47" s="71"/>
+      <c r="E47" s="72"/>
+      <c r="F47" s="73"/>
+      <c r="G47" s="72"/>
+      <c r="H47" s="71"/>
+      <c r="I47" s="71"/>
+      <c r="J47" s="74"/>
+      <c r="K47" s="75"/>
+    </row>
+    <row r="48" spans="1:11" s="61" customFormat="1" ht="15" customHeight="1">
+      <c r="A48" s="69"/>
+      <c r="B48" s="70"/>
+      <c r="C48" s="71"/>
+      <c r="D48" s="71"/>
+      <c r="E48" s="72"/>
+      <c r="F48" s="73"/>
+      <c r="G48" s="72"/>
+      <c r="H48" s="71"/>
+      <c r="I48" s="71"/>
+      <c r="J48" s="74"/>
+      <c r="K48" s="75"/>
     </row>
     <row r="49" spans="1:11" ht="15" customHeight="1">
       <c r="A49" s="19"/>
@@ -17985,16 +17966,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B4:N4"/>
+    <mergeCell ref="B2:N2"/>
     <mergeCell ref="B18:N18"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="G6:K6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B4:N4"/>
-    <mergeCell ref="B2:N2"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Click and enter a value from the list of items (Low, Medium, or High)" sqref="I29:I33 I45:I48 I40:I43 I24:I27 I35:I38">
@@ -18005,6 +17986,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
-  <pageSetup fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="62" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>